<commit_message>
update test case and update mobile
</commit_message>
<xml_diff>
--- a/Test case/tase case.xlsx
+++ b/Test case/tase case.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="630" windowWidth="24615" windowHeight="13485" activeTab="1"/>
+    <workbookView xWindow="270" yWindow="630" windowWidth="24615" windowHeight="13485"/>
   </bookViews>
   <sheets>
     <sheet name="website" sheetId="1" r:id="rId1"/>
@@ -1557,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:O1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2994,7 +2994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>

</xml_diff>